<commit_message>
Update report Add some page Add some data info
</commit_message>
<xml_diff>
--- a/Report/error_data.xlsx
+++ b/Report/error_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="4980" yWindow="500" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="error_data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>symbol</t>
   </si>
@@ -50,67 +50,70 @@
     <t>Normalized MSE</t>
   </si>
   <si>
-    <t>0001.HK</t>
+    <t>0001.HK.csv</t>
   </si>
   <si>
-    <t>0002.HK</t>
+    <t>0002.HK.csv</t>
   </si>
   <si>
-    <t>0004.HK</t>
+    <t>0003.HK.csv</t>
   </si>
   <si>
-    <t>0005.HK</t>
+    <t>0004.HK.csv</t>
   </si>
   <si>
-    <t>0006.HK</t>
+    <t>0005.HK.csv</t>
   </si>
   <si>
-    <t>0010.HK</t>
+    <t>0006.HK.csv</t>
   </si>
   <si>
-    <t>0011.HK</t>
+    <t>0010.HK.csv</t>
   </si>
   <si>
-    <t>0012.HK</t>
+    <t>0011.HK.csv</t>
   </si>
   <si>
-    <t>0013.HK</t>
+    <t>0012.HK.csv</t>
   </si>
   <si>
-    <t>0014.HK</t>
+    <t>0013.HK.csv</t>
   </si>
   <si>
-    <t>0016.HK</t>
+    <t>0014.HK.csv</t>
   </si>
   <si>
-    <t>0019.HK</t>
+    <t>0016.HK.csv</t>
   </si>
   <si>
-    <t>0020.HK</t>
+    <t>0019.HK.csv</t>
   </si>
   <si>
-    <t>0023.HK</t>
+    <t>0020.HK.csv</t>
   </si>
   <si>
-    <t>0026.HK</t>
+    <t>0023.HK.csv</t>
   </si>
   <si>
-    <t>0027.HK</t>
+    <t>0026.HK.csv</t>
   </si>
   <si>
-    <t>0041.HK</t>
+    <t>0027.HK.csv</t>
   </si>
   <si>
-    <t>0044.HK</t>
+    <t>0041.HK.csv</t>
   </si>
   <si>
-    <t>0053.HK</t>
+    <t>0044.HK.csv</t>
   </si>
   <si>
-    <t>0054.HK</t>
+    <t>0053.HK.csv</t>
   </si>
   <si>
-    <t>0062.HK</t>
+    <t>0054.HK.csv</t>
+  </si>
+  <si>
+    <t>0062.HK.csv</t>
   </si>
 </sst>
 </file>
@@ -279,67 +282,67 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0001.HK</c:v>
+                  <c:v>0001.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0002.HK</c:v>
+                  <c:v>0002.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0004.HK</c:v>
+                  <c:v>0003.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0005.HK</c:v>
+                  <c:v>0004.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0006.HK</c:v>
+                  <c:v>0005.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0010.HK</c:v>
+                  <c:v>0006.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0011.HK</c:v>
+                  <c:v>0010.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0012.HK</c:v>
+                  <c:v>0011.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0013.HK</c:v>
+                  <c:v>0012.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0014.HK</c:v>
+                  <c:v>0013.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0016.HK</c:v>
+                  <c:v>0014.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0019.HK</c:v>
+                  <c:v>0016.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0020.HK</c:v>
+                  <c:v>0019.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0023.HK</c:v>
+                  <c:v>0020.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0026.HK</c:v>
+                  <c:v>0023.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0027.HK</c:v>
+                  <c:v>0026.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0041.HK</c:v>
+                  <c:v>0027.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0044.HK</c:v>
+                  <c:v>0041.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0053.HK</c:v>
+                  <c:v>0044.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0054.HK</c:v>
+                  <c:v>0053.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0062.HK</c:v>
+                  <c:v>0054.HK.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -348,70 +351,70 @@
             <c:numRef>
               <c:f>error_data!$C$2:$C$22</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.0169435613311</c:v>
+                  <c:v>0.0147153668586</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00967220261695</c:v>
+                  <c:v>0.00821545882022</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0197731859103</c:v>
+                  <c:v>0.0912652056621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0138085220966</c:v>
+                  <c:v>0.017184484707</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0139607541811</c:v>
+                  <c:v>0.0125810958578</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0181173137092</c:v>
+                  <c:v>0.0122171116326</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0126703551497</c:v>
+                  <c:v>0.0171580609869</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0193908076803</c:v>
+                  <c:v>0.0109098944227</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0144329824007</c:v>
+                  <c:v>0.0165046489167</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0342077296248</c:v>
+                  <c:v>0.0133212656735</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.015414750458</c:v>
+                  <c:v>0.0375519792843</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0133649330615</c:v>
+                  <c:v>0.0132331857964</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.041066303142</c:v>
+                  <c:v>0.0119398877211</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0231297162294</c:v>
+                  <c:v>0.0426709744493</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.013052407146</c:v>
+                  <c:v>0.0218273136922</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0508435511579</c:v>
+                  <c:v>0.0129179634902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0571895898042</c:v>
+                  <c:v>0.0504280965191</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0109265903419</c:v>
+                  <c:v>0.058963230739</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.00739477053251</c:v>
+                  <c:v>0.00898221748786</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0420377851818</c:v>
+                  <c:v>0.00618900811818</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0395704999935</c:v>
+                  <c:v>0.0431097351296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -447,67 +450,67 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0001.HK</c:v>
+                  <c:v>0001.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0002.HK</c:v>
+                  <c:v>0002.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0004.HK</c:v>
+                  <c:v>0003.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0005.HK</c:v>
+                  <c:v>0004.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0006.HK</c:v>
+                  <c:v>0005.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0010.HK</c:v>
+                  <c:v>0006.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0011.HK</c:v>
+                  <c:v>0010.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0012.HK</c:v>
+                  <c:v>0011.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0013.HK</c:v>
+                  <c:v>0012.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0014.HK</c:v>
+                  <c:v>0013.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0016.HK</c:v>
+                  <c:v>0014.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0019.HK</c:v>
+                  <c:v>0016.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0020.HK</c:v>
+                  <c:v>0019.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0023.HK</c:v>
+                  <c:v>0020.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0026.HK</c:v>
+                  <c:v>0023.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0027.HK</c:v>
+                  <c:v>0026.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0041.HK</c:v>
+                  <c:v>0027.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0044.HK</c:v>
+                  <c:v>0041.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0053.HK</c:v>
+                  <c:v>0044.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0054.HK</c:v>
+                  <c:v>0053.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0062.HK</c:v>
+                  <c:v>0054.HK.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -516,70 +519,70 @@
             <c:numRef>
               <c:f>error_data!$F$2:$F$22</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.0169435613311</c:v>
+                  <c:v>0.0146161507557</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00967220261695</c:v>
+                  <c:v>0.00832073183653</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0197731859103</c:v>
+                  <c:v>0.0116521546846</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0138085220966</c:v>
+                  <c:v>0.0170215411258</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0139607541811</c:v>
+                  <c:v>0.0126180151051</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0181173137092</c:v>
+                  <c:v>0.0124471062134</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0126703551497</c:v>
+                  <c:v>0.0160947021817</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0193908076803</c:v>
+                  <c:v>0.0110899873053</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0144329824007</c:v>
+                  <c:v>0.0165275803973</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0342077296248</c:v>
+                  <c:v>0.0133143975886</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.015414750458</c:v>
+                  <c:v>0.0125921671482</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0133649330615</c:v>
+                  <c:v>0.0134561777464</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.041066303142</c:v>
+                  <c:v>0.0122103257866</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0231297162294</c:v>
+                  <c:v>0.0166922232673</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.013052407146</c:v>
+                  <c:v>0.014326406372</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0508435511579</c:v>
+                  <c:v>0.0131689452844</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0571895898042</c:v>
+                  <c:v>0.0300418338069</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0109265903419</c:v>
+                  <c:v>0.0125795305073</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.00739477053251</c:v>
+                  <c:v>0.00934128875996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0420377851818</c:v>
+                  <c:v>0.00617929269897</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0395704999935</c:v>
+                  <c:v>0.011010183392</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,11 +598,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2143703872"/>
-        <c:axId val="-2112472960"/>
+        <c:axId val="2145548704"/>
+        <c:axId val="-2089192176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2143703872"/>
+        <c:axId val="2145548704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112472960"/>
+        <c:crossAx val="-2089192176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -649,7 +652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112472960"/>
+        <c:axId val="-2089192176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -713,7 +716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143703872"/>
+        <c:crossAx val="2145548704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -904,67 +907,67 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0001.HK</c:v>
+                  <c:v>0001.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0002.HK</c:v>
+                  <c:v>0002.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0004.HK</c:v>
+                  <c:v>0003.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0005.HK</c:v>
+                  <c:v>0004.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0006.HK</c:v>
+                  <c:v>0005.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0010.HK</c:v>
+                  <c:v>0006.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0011.HK</c:v>
+                  <c:v>0010.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0012.HK</c:v>
+                  <c:v>0011.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0013.HK</c:v>
+                  <c:v>0012.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0014.HK</c:v>
+                  <c:v>0013.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0016.HK</c:v>
+                  <c:v>0014.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0019.HK</c:v>
+                  <c:v>0016.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0020.HK</c:v>
+                  <c:v>0019.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0023.HK</c:v>
+                  <c:v>0020.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0026.HK</c:v>
+                  <c:v>0023.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0027.HK</c:v>
+                  <c:v>0026.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0041.HK</c:v>
+                  <c:v>0027.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0044.HK</c:v>
+                  <c:v>0041.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0053.HK</c:v>
+                  <c:v>0044.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0054.HK</c:v>
+                  <c:v>0053.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0062.HK</c:v>
+                  <c:v>0054.HK.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -976,67 +979,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.74846465698</c:v>
+                  <c:v>1.52221931328</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.637420836243</c:v>
+                  <c:v>0.543114385205</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.991872793524</c:v>
+                  <c:v>1.64455213147</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.915774700234</c:v>
+                  <c:v>0.86414667098</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.00083891555</c:v>
+                  <c:v>0.833582322854</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.601914964077</c:v>
+                  <c:v>0.874961845458</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7561435383</c:v>
+                  <c:v>0.586654208096</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.03937199864</c:v>
+                  <c:v>1.51555977609</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.46047919804</c:v>
+                  <c:v>0.883255724482</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.18657309667</c:v>
+                  <c:v>1.3505573687</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.65793763118</c:v>
+                  <c:v>1.30449325081</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.23190077711</c:v>
+                  <c:v>1.4324870346</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.51592402682</c:v>
+                  <c:v>1.1109038684</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.692492826652</c:v>
+                  <c:v>1.58054203342</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.06276069334</c:v>
+                  <c:v>0.661576157476</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.99274514639</c:v>
+                  <c:v>1.04762865843</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.52027322597</c:v>
+                  <c:v>1.98158855292</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.775843220758</c:v>
+                  <c:v>1.56970434646</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.65932189582</c:v>
+                  <c:v>0.640656029957</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.15696858052</c:v>
+                  <c:v>0.552769871397</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.719672063683</c:v>
+                  <c:v>1.1859575927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1072,67 +1075,67 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0001.HK</c:v>
+                  <c:v>0001.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0002.HK</c:v>
+                  <c:v>0002.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0004.HK</c:v>
+                  <c:v>0003.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0005.HK</c:v>
+                  <c:v>0004.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0006.HK</c:v>
+                  <c:v>0005.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0010.HK</c:v>
+                  <c:v>0006.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0011.HK</c:v>
+                  <c:v>0010.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0012.HK</c:v>
+                  <c:v>0011.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0013.HK</c:v>
+                  <c:v>0012.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0014.HK</c:v>
+                  <c:v>0013.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0016.HK</c:v>
+                  <c:v>0014.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0019.HK</c:v>
+                  <c:v>0016.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0020.HK</c:v>
+                  <c:v>0019.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0023.HK</c:v>
+                  <c:v>0020.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0026.HK</c:v>
+                  <c:v>0023.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0027.HK</c:v>
+                  <c:v>0026.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0041.HK</c:v>
+                  <c:v>0027.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0044.HK</c:v>
+                  <c:v>0041.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0053.HK</c:v>
+                  <c:v>0044.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0054.HK</c:v>
+                  <c:v>0053.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0062.HK</c:v>
+                  <c:v>0054.HK.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1144,67 +1147,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.51021577303</c:v>
+                  <c:v>1.51271192687</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.549738775667</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.205992212163</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.848853473786</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.837346603499</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.890895776106</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.537995591112</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.54105559291</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.885818909174</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1.35007780775</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.43095274802</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>1.45950421991</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1.13891095021</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.614725642348</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.42308114323</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1.06448255836</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1.13656883636</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.332420248513</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>0.66853521058</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.552360397179</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.297003175753</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.182803100585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,11 +1223,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2102169872"/>
-        <c:axId val="-2123166864"/>
+        <c:axId val="-2095769888"/>
+        <c:axId val="-2104887360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2102169872"/>
+        <c:axId val="-2095769888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1266,7 +1269,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123166864"/>
+        <c:crossAx val="-2104887360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1274,7 +1277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123166864"/>
+        <c:axId val="-2104887360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1327,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2102169872"/>
+        <c:crossAx val="-2095769888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1512,67 +1515,67 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0001.HK</c:v>
+                  <c:v>0001.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0002.HK</c:v>
+                  <c:v>0002.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0004.HK</c:v>
+                  <c:v>0003.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0005.HK</c:v>
+                  <c:v>0004.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0006.HK</c:v>
+                  <c:v>0005.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0010.HK</c:v>
+                  <c:v>0006.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0011.HK</c:v>
+                  <c:v>0010.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0012.HK</c:v>
+                  <c:v>0011.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0013.HK</c:v>
+                  <c:v>0012.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0014.HK</c:v>
+                  <c:v>0013.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0016.HK</c:v>
+                  <c:v>0014.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0019.HK</c:v>
+                  <c:v>0016.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0020.HK</c:v>
+                  <c:v>0019.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0023.HK</c:v>
+                  <c:v>0020.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0026.HK</c:v>
+                  <c:v>0023.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0027.HK</c:v>
+                  <c:v>0026.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0041.HK</c:v>
+                  <c:v>0027.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0044.HK</c:v>
+                  <c:v>0041.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0053.HK</c:v>
+                  <c:v>0044.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0054.HK</c:v>
+                  <c:v>0053.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0062.HK</c:v>
+                  <c:v>0054.HK.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1584,67 +1587,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>5.22463058846</c:v>
+                  <c:v>4.20991515734</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.648429560952</c:v>
+                  <c:v>0.47288044013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.51971057923</c:v>
+                  <c:v>2.81304268979</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4367441893</c:v>
+                  <c:v>1.14678557629</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.64040247761</c:v>
+                  <c:v>1.2275067</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.608762212335</c:v>
+                  <c:v>1.32036627666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.05150307805</c:v>
+                  <c:v>0.577358975226</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.84289096242</c:v>
+                  <c:v>4.60104402339</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.87226575422</c:v>
+                  <c:v>1.38459589532</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.74476903284</c:v>
+                  <c:v>3.32235364359</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.94348612386</c:v>
+                  <c:v>1.99346310902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.68407587485</c:v>
+                  <c:v>3.62221394046</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.05722437513</c:v>
+                  <c:v>2.15006007129</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.688886905526</c:v>
+                  <c:v>3.1142486857</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.37006294183</c:v>
+                  <c:v>0.623583991691</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.13170927051</c:v>
+                  <c:v>2.61965733839</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.56291713532</c:v>
+                  <c:v>5.79410857266</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.14660771514</c:v>
+                  <c:v>2.67282408419</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.910605616236</c:v>
+                  <c:v>0.733904169964</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.52097222561</c:v>
+                  <c:v>0.586828054431</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.610429673338</c:v>
+                  <c:v>1.54619925638</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,67 +1683,67 @@
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0001.HK</c:v>
+                  <c:v>0001.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0002.HK</c:v>
+                  <c:v>0002.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0004.HK</c:v>
+                  <c:v>0003.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0005.HK</c:v>
+                  <c:v>0004.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0006.HK</c:v>
+                  <c:v>0005.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0010.HK</c:v>
+                  <c:v>0006.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0011.HK</c:v>
+                  <c:v>0010.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0012.HK</c:v>
+                  <c:v>0011.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0013.HK</c:v>
+                  <c:v>0012.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0014.HK</c:v>
+                  <c:v>0013.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0016.HK</c:v>
+                  <c:v>0014.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0019.HK</c:v>
+                  <c:v>0016.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0020.HK</c:v>
+                  <c:v>0019.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0023.HK</c:v>
+                  <c:v>0020.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0026.HK</c:v>
+                  <c:v>0023.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0027.HK</c:v>
+                  <c:v>0026.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0041.HK</c:v>
+                  <c:v>0027.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0044.HK</c:v>
+                  <c:v>0041.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0053.HK</c:v>
+                  <c:v>0044.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0054.HK</c:v>
+                  <c:v>0053.HK.csv</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0062.HK</c:v>
+                  <c:v>0054.HK.csv</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1752,67 +1755,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>4.02338518638</c:v>
+                  <c:v>4.02662519407</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.479536794741</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.0840293947855</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.06726577217</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.19615633681</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.34591602878</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.495264617697</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>4.58334495816</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1.3623955613</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3.22873311914</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.321072170713</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>3.64609275483</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>2.18384882868</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.606142183864</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.301192032314</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>2.41836052511</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>2.11887545274</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.19259952644</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>0.736097481098</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.560240077036</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.144845325179</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0706212089273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1828,11 +1831,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2096702816"/>
-        <c:axId val="-2112666640"/>
+        <c:axId val="-2105317408"/>
+        <c:axId val="-2107414816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2096702816"/>
+        <c:axId val="-2105317408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112666640"/>
+        <c:crossAx val="-2107414816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1883,7 +1886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112666640"/>
+        <c:axId val="-2107414816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,7 +1936,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096702816"/>
+        <c:crossAx val="-2105317408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4001,10 +4004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:G22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4020,7 +4023,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -4029,7 +4032,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -4041,22 +4044,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.74846465698</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.6943561331100001E-2</v>
+        <v>1.5222193132799999</v>
+      </c>
+      <c r="C2">
+        <v>1.4715366858600001E-2</v>
       </c>
       <c r="D2">
-        <v>5.2246305884600002</v>
+        <v>4.2099151573400002</v>
       </c>
       <c r="E2">
-        <v>1.5102157730300001</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.6943561331100001E-2</v>
+        <v>1.51271192687</v>
+      </c>
+      <c r="F2">
+        <v>1.46161507557E-2</v>
       </c>
       <c r="G2">
-        <v>4.0233851863799996</v>
+        <v>4.0266251940700002</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -4064,19 +4067,19 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.63742083624300006</v>
-      </c>
-      <c r="C3" s="1">
-        <v>9.6722026169499993E-3</v>
+        <v>0.54311438520499999</v>
+      </c>
+      <c r="C3">
+        <v>8.2154588202199997E-3</v>
       </c>
       <c r="D3">
-        <v>0.64842956095199999</v>
+        <v>0.47288044013000002</v>
       </c>
       <c r="E3">
         <v>0.54973877566700002</v>
       </c>
-      <c r="F3" s="1">
-        <v>9.6722026169499993E-3</v>
+      <c r="F3">
+        <v>8.3207318365299994E-3</v>
       </c>
       <c r="G3">
         <v>0.47953679474100003</v>
@@ -4087,22 +4090,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.99187279352400004</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.9773185910300001E-2</v>
+        <v>1.64455213147</v>
+      </c>
+      <c r="C4">
+        <v>9.1265205662100002E-2</v>
       </c>
       <c r="D4">
-        <v>1.5197105792300001</v>
+        <v>2.8130426897900001</v>
       </c>
       <c r="E4">
-        <v>0.84885347378599996</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1.9773185910300001E-2</v>
+        <v>0.20599221216300001</v>
+      </c>
+      <c r="F4">
+        <v>1.16521546846E-2</v>
       </c>
       <c r="G4">
-        <v>1.0672657721700001</v>
+        <v>8.4029394785500006E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4110,22 +4113,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.91577470023399998</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.3808522096600001E-2</v>
+        <v>0.86414667097999998</v>
+      </c>
+      <c r="C5">
+        <v>1.7184484707E-2</v>
       </c>
       <c r="D5">
-        <v>1.4367441892999999</v>
+        <v>1.1467855762900001</v>
       </c>
       <c r="E5">
-        <v>0.83734660349900003</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1.3808522096600001E-2</v>
+        <v>0.84885347378599996</v>
+      </c>
+      <c r="F5">
+        <v>1.70215411258E-2</v>
       </c>
       <c r="G5">
-        <v>1.1961563368100001</v>
+        <v>1.0672657721700001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -4133,22 +4136,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>1.0008389155499999</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1.39607541811E-2</v>
+        <v>0.83358232285400002</v>
+      </c>
+      <c r="C6">
+        <v>1.25810958578E-2</v>
       </c>
       <c r="D6">
-        <v>1.6404024776099999</v>
+        <v>1.2275067</v>
       </c>
       <c r="E6">
-        <v>0.89089577610600001</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.39607541811E-2</v>
+        <v>0.83734660349900003</v>
+      </c>
+      <c r="F6">
+        <v>1.26180151051E-2</v>
       </c>
       <c r="G6">
-        <v>1.3459160287800001</v>
+        <v>1.1961563368100001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4156,22 +4159,22 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.60191496407699996</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.81173137092E-2</v>
+        <v>0.87496184545800004</v>
+      </c>
+      <c r="C7">
+        <v>1.2217111632599999E-2</v>
       </c>
       <c r="D7">
-        <v>0.60876221233500005</v>
+        <v>1.3203662766599999</v>
       </c>
       <c r="E7">
-        <v>0.53799559111200002</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.81173137092E-2</v>
+        <v>0.89089577610600001</v>
+      </c>
+      <c r="F7">
+        <v>1.24471062134E-2</v>
       </c>
       <c r="G7">
-        <v>0.49526461769699998</v>
+        <v>1.3459160287800001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -4179,22 +4182,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>1.7561435382999999</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.26703551497E-2</v>
+        <v>0.586654208096</v>
+      </c>
+      <c r="C8">
+        <v>1.7158060986899999E-2</v>
       </c>
       <c r="D8">
-        <v>6.0515030780499997</v>
+        <v>0.57735897522599999</v>
       </c>
       <c r="E8">
-        <v>1.54105559291</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1.26703551497E-2</v>
+        <v>0.53799559111200002</v>
+      </c>
+      <c r="F8">
+        <v>1.6094702181700001E-2</v>
       </c>
       <c r="G8">
-        <v>4.5833449581599996</v>
+        <v>0.49526461769699998</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4202,22 +4205,22 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>1.0393719986400001</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1.93908076803E-2</v>
+        <v>1.5155597760899999</v>
+      </c>
+      <c r="C9">
+        <v>1.09098944227E-2</v>
       </c>
       <c r="D9">
-        <v>1.8428909624200001</v>
+        <v>4.6010440233900001</v>
       </c>
       <c r="E9">
-        <v>0.88581890917399997</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1.93908076803E-2</v>
+        <v>1.54105559291</v>
+      </c>
+      <c r="F9">
+        <v>1.10899873053E-2</v>
       </c>
       <c r="G9">
-        <v>1.3623955613000001</v>
+        <v>4.5833449581599996</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -4225,22 +4228,22 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>1.46047919804</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1.44329824007E-2</v>
+        <v>0.88325572448199996</v>
+      </c>
+      <c r="C10">
+        <v>1.6504648916700001E-2</v>
       </c>
       <c r="D10">
-        <v>3.8722657542199999</v>
+        <v>1.3845958953199999</v>
       </c>
       <c r="E10">
-        <v>1.35007780775</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1.44329824007E-2</v>
+        <v>0.88581890917399997</v>
+      </c>
+      <c r="F10">
+        <v>1.6527580397299999E-2</v>
       </c>
       <c r="G10">
-        <v>3.2287331191400002</v>
+        <v>1.3623955613000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4248,22 +4251,22 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>1.1865730966700001</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3.4207729624800003E-2</v>
+        <v>1.3505573687000001</v>
+      </c>
+      <c r="C11">
+        <v>1.3321265673499999E-2</v>
       </c>
       <c r="D11">
-        <v>1.7447690328400001</v>
+        <v>3.3223536435900001</v>
       </c>
       <c r="E11">
-        <v>0.43095274802</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3.4207729624800003E-2</v>
+        <v>1.35007780775</v>
+      </c>
+      <c r="F11">
+        <v>1.3314397588600001E-2</v>
       </c>
       <c r="G11">
-        <v>0.32107217071299998</v>
+        <v>3.2287331191400002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4271,22 +4274,22 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>1.65793763118</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1.5414750458E-2</v>
+        <v>1.30449325081</v>
+      </c>
+      <c r="C12">
+        <v>3.7551979284299999E-2</v>
       </c>
       <c r="D12">
-        <v>4.9434861238599996</v>
+        <v>1.9934631090199999</v>
       </c>
       <c r="E12">
-        <v>1.4595042199099999</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.5414750458E-2</v>
+        <v>0.43095274802</v>
+      </c>
+      <c r="F12">
+        <v>1.25921671482E-2</v>
       </c>
       <c r="G12">
-        <v>3.6460927548300002</v>
+        <v>0.32107217071299998</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4294,22 +4297,22 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>1.2319007771099999</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1.33649330615E-2</v>
+        <v>1.4324870346</v>
+      </c>
+      <c r="C13">
+        <v>1.32331857964E-2</v>
       </c>
       <c r="D13">
-        <v>2.68407587485</v>
+        <v>3.62221394046</v>
       </c>
       <c r="E13">
-        <v>1.1389109502100001</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1.33649330615E-2</v>
+        <v>1.4595042199099999</v>
+      </c>
+      <c r="F13">
+        <v>1.3456177746400001E-2</v>
       </c>
       <c r="G13">
-        <v>2.18384882868</v>
+        <v>3.6460927548300002</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -4317,22 +4320,22 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>1.51592402682</v>
-      </c>
-      <c r="C14" s="1">
-        <v>4.1066303142E-2</v>
+        <v>1.1109038684000001</v>
+      </c>
+      <c r="C14">
+        <v>1.1939887721100001E-2</v>
       </c>
       <c r="D14">
-        <v>3.0572243751300001</v>
+        <v>2.15006007129</v>
       </c>
       <c r="E14">
-        <v>0.61472564234799998</v>
-      </c>
-      <c r="F14" s="1">
-        <v>4.1066303142E-2</v>
+        <v>1.1389109502100001</v>
+      </c>
+      <c r="F14">
+        <v>1.22103257866E-2</v>
       </c>
       <c r="G14">
-        <v>0.60614218386399998</v>
+        <v>2.18384882868</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4340,22 +4343,22 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.69249282665199996</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2.3129716229400001E-2</v>
+        <v>1.58054203342</v>
+      </c>
+      <c r="C15">
+        <v>4.26709744493E-2</v>
       </c>
       <c r="D15">
-        <v>0.68888690552599996</v>
+        <v>3.1142486856999998</v>
       </c>
       <c r="E15">
-        <v>0.42308114323000001</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2.3129716229400001E-2</v>
+        <v>0.61472564234799998</v>
+      </c>
+      <c r="F15">
+        <v>1.6692223267300001E-2</v>
       </c>
       <c r="G15">
-        <v>0.30119203231399999</v>
+        <v>0.60614218386399998</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -4363,22 +4366,22 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>1.06276069334</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1.3052407146000001E-2</v>
+        <v>0.66157615747599996</v>
+      </c>
+      <c r="C16">
+        <v>2.18273136922E-2</v>
       </c>
       <c r="D16">
-        <v>3.3700629418300001</v>
+        <v>0.62358399169099998</v>
       </c>
       <c r="E16">
-        <v>1.0644825583599999</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1.3052407146000001E-2</v>
+        <v>0.42308114323000001</v>
+      </c>
+      <c r="F16">
+        <v>1.4326406372E-2</v>
       </c>
       <c r="G16">
-        <v>2.4183605251100002</v>
+        <v>0.30119203231399999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4386,22 +4389,22 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>1.9927451463900001</v>
-      </c>
-      <c r="C17" s="1">
-        <v>5.0843551157899999E-2</v>
+        <v>1.0476286584300001</v>
+      </c>
+      <c r="C17">
+        <v>1.29179634902E-2</v>
       </c>
       <c r="D17">
-        <v>6.13170927051</v>
+        <v>2.6196573383900001</v>
       </c>
       <c r="E17">
-        <v>1.1365688363599999</v>
-      </c>
-      <c r="F17" s="1">
-        <v>5.0843551157899999E-2</v>
+        <v>1.0644825583599999</v>
+      </c>
+      <c r="F17">
+        <v>1.31689452844E-2</v>
       </c>
       <c r="G17">
-        <v>2.1188754527400002</v>
+        <v>2.4183605251100002</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -4409,22 +4412,22 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>1.52027322597</v>
-      </c>
-      <c r="C18" s="1">
-        <v>5.7189589804199997E-2</v>
+        <v>1.9815885529199999</v>
+      </c>
+      <c r="C18">
+        <v>5.0428096519099998E-2</v>
       </c>
       <c r="D18">
-        <v>2.5629171353200002</v>
+        <v>5.7941085726599999</v>
       </c>
       <c r="E18">
-        <v>0.33242024851300001</v>
-      </c>
-      <c r="F18" s="1">
-        <v>5.7189589804199997E-2</v>
+        <v>1.1365688363599999</v>
+      </c>
+      <c r="F18">
+        <v>3.0041833806899999E-2</v>
       </c>
       <c r="G18">
-        <v>0.19259952644</v>
+        <v>2.1188754527400002</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4432,22 +4435,22 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.77584322075800005</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1.09265903419E-2</v>
+        <v>1.56970434646</v>
+      </c>
+      <c r="C19">
+        <v>5.8963230738999999E-2</v>
       </c>
       <c r="D19">
-        <v>1.14660771514</v>
+        <v>2.6728240841900002</v>
       </c>
       <c r="E19">
-        <v>0.66853521057999998</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.09265903419E-2</v>
+        <v>0.33242024851300001</v>
+      </c>
+      <c r="F19">
+        <v>1.2579530507300001E-2</v>
       </c>
       <c r="G19">
-        <v>0.73609748109799999</v>
+        <v>0.19259952644</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -4455,22 +4458,22 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.65932189582</v>
-      </c>
-      <c r="C20" s="1">
-        <v>7.3947705325099998E-3</v>
+        <v>0.640656029957</v>
+      </c>
+      <c r="C20">
+        <v>8.9822174878599996E-3</v>
       </c>
       <c r="D20">
-        <v>0.910605616236</v>
+        <v>0.73390416996399999</v>
       </c>
       <c r="E20">
-        <v>0.55236039717899998</v>
-      </c>
-      <c r="F20" s="1">
-        <v>7.3947705325099998E-3</v>
+        <v>0.66853521057999998</v>
+      </c>
+      <c r="F20">
+        <v>9.3412887599600009E-3</v>
       </c>
       <c r="G20">
-        <v>0.56024007703599998</v>
+        <v>0.73609748109799999</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -4478,22 +4481,22 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>1.1569685805200001</v>
-      </c>
-      <c r="C21" s="1">
-        <v>4.20377851818E-2</v>
+        <v>0.55276987139699996</v>
+      </c>
+      <c r="C21">
+        <v>6.1890081181799998E-3</v>
       </c>
       <c r="D21">
-        <v>1.52097222561</v>
+        <v>0.58682805443099995</v>
       </c>
       <c r="E21">
-        <v>0.297003175753</v>
-      </c>
-      <c r="F21" s="1">
-        <v>4.20377851818E-2</v>
+        <v>0.55236039717899998</v>
+      </c>
+      <c r="F21">
+        <v>6.1792926989700002E-3</v>
       </c>
       <c r="G21">
-        <v>0.14484532517900001</v>
+        <v>0.56024007703599998</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -4501,21 +4504,44 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.71967206368299996</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3.95704999935E-2</v>
+        <v>1.1859575926999999</v>
+      </c>
+      <c r="C22">
+        <v>4.3109735129600001E-2</v>
       </c>
       <c r="D22">
-        <v>0.61042967333800002</v>
+        <v>1.54619925638</v>
       </c>
       <c r="E22">
+        <v>0.297003175753</v>
+      </c>
+      <c r="F22">
+        <v>1.1010183392E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.14484532517900001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>0.71478826783100002</v>
+      </c>
+      <c r="C23">
+        <v>3.9397365779500003E-2</v>
+      </c>
+      <c r="D23">
+        <v>0.58245921158799996</v>
+      </c>
+      <c r="E23">
         <v>0.18280310058499999</v>
       </c>
-      <c r="F22" s="1">
-        <v>3.95704999935E-2</v>
-      </c>
-      <c r="G22">
+      <c r="F23">
+        <v>9.9381003854800004E-3</v>
+      </c>
+      <c r="G23">
         <v>7.0621208927300005E-2</v>
       </c>
     </row>

</xml_diff>